<commit_message>
Touch is working -Delays Added
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23102" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23510" uniqueCount="223">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1870,7 +1870,7 @@
         <v>45</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J4" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
Splash Screen Edited & Bug fixed
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23510" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23918" uniqueCount="225">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -684,6 +684,12 @@
   </si>
   <si>
     <t xml:space="preserve">MODE_SOIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRECITEST     FW412</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRECITEST     FW403</t>
   </si>
 </sst>
 </file>
@@ -2993,7 +2999,7 @@
         <v>44</v>
       </c>
       <c r="F49" t="s">
-        <v>197</v>
+        <v>223</v>
       </c>
       <c r="G49" t="s">
         <v>49</v>
@@ -3013,7 +3019,7 @@
         <v>44</v>
       </c>
       <c r="F50" t="s">
-        <v>199</v>
+        <v>224</v>
       </c>
       <c r="G50" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Ranges are correct & has Very Low
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23918" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24326" uniqueCount="226">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -690,6 +690,9 @@
   </si>
   <si>
     <t xml:space="preserve">PRECITEST     FW403</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRECITEST     PT-012</t>
   </si>
 </sst>
 </file>
@@ -2999,7 +3002,7 @@
         <v>44</v>
       </c>
       <c r="F49" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="G49" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Remove the HOLD and add History Button
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24326" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24734" uniqueCount="227">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -693,6 +693,9 @@
   </si>
   <si>
     <t xml:space="preserve">PRECITEST     PT-012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">History</t>
   </si>
 </sst>
 </file>
@@ -2189,7 +2192,7 @@
         <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5">

</xml_diff>